<commit_message>
:star: Add equity information and key creation
</commit_message>
<xml_diff>
--- a/url_base2.xlsx
+++ b/url_base2.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive - larrainvial.com\LV\Web Traffic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Desarrollo LV\Repositorios\Data alternativa\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -46,7 +46,7 @@
     <definedName name="IQ_YTD">3000</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511" iterate="1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="703">
   <si>
     <t>Ticker CIQ</t>
   </si>
@@ -160,9 +160,6 @@
     <t>BMV:FEMSA UBD</t>
   </si>
   <si>
-    <t>NASDAQ:STNE</t>
-  </si>
-  <si>
     <t>https://www.stone.co/</t>
   </si>
   <si>
@@ -556,9 +553,6 @@
     <t>https://www.megacable.com.mx/</t>
   </si>
   <si>
-    <t>BOVESPA:BIDI4</t>
-  </si>
-  <si>
     <t>https://www.bancointer.com.br/</t>
   </si>
   <si>
@@ -805,12 +799,6 @@
     <t>BMV:TERRA 13</t>
   </si>
   <si>
-    <t>BOVESPA:PETZ3</t>
-  </si>
-  <si>
-    <t>https://www.petz.com.br/</t>
-  </si>
-  <si>
     <t>SNSE:AFPCAPITAL</t>
   </si>
   <si>
@@ -2171,12 +2159,18 @@
   </si>
   <si>
     <t>NYSE:AGRO</t>
+  </si>
+  <si>
+    <t>NasdaqGS:STNE</t>
+  </si>
+  <si>
+    <t>BOVESPA:BIDI11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2515,19 +2509,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B641"/>
+  <dimension ref="A1:B640"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="A195" sqref="A195:XFD195"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2535,60 +2529,60 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
@@ -2596,33 +2590,33 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -2630,17 +2624,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
@@ -2648,12 +2642,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>28</v>
       </c>
@@ -2661,3268 +2655,3260 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="2" t="s">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="2" t="s">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="2" t="s">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
+      <c r="B30" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="3" t="s">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="2" t="s">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="2" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="2" t="s">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="2" t="s">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="2" t="s">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
+      <c r="B42" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B45" s="2" t="s">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B46" s="2" t="s">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="2" t="s">
+      <c r="B48" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="3" t="s">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B49" s="2" t="s">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B50" s="2" t="s">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" s="2" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="2" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="2" t="s">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B54" s="2" t="s">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B55" s="2" t="s">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B56" s="2" t="s">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="2" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" s="2" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" s="2" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="2" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B61" s="2" t="s">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" s="2" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" s="2" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" s="2" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B65" s="2" t="s">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66" s="2" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" s="2" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B68" s="2" t="s">
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B69" s="2" t="s">
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70" s="2" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" s="2" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B72" s="2" t="s">
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" s="2" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A74" s="2" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B75" s="2" t="s">
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76" s="2" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B77" s="2" t="s">
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A78" s="2" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A79" s="2" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A80" s="2" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B81" s="2" t="s">
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" s="2" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A83" s="2" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" s="2" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" s="2" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" s="2" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" s="2" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" s="2" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" s="2" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A90" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B90" s="2" t="s">
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91" s="2" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92" s="2" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B93" s="2" t="s">
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" s="2" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95" s="2" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B96" s="2" t="s">
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" s="2" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98" s="2" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A99" s="2" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100" s="2" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" s="2" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B102" s="2" t="s">
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" s="2" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A104" s="2" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" s="2" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" s="2" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107" s="2" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A108" s="2" t="s">
+      <c r="B108" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B108" s="2" t="s">
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109" s="2" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" s="2" t="s">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" s="2" t="s">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A112" s="2" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A113" s="2" t="s">
+      <c r="B113" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B113" s="2" t="s">
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A114" s="2" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A115" s="2" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A116" s="2" t="s">
+      <c r="B116" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B116" s="2" t="s">
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A117" s="2" t="s">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A118" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B118" s="2" t="s">
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A119" s="2" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A120" s="2" t="s">
+      <c r="B120" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B120" s="2" t="s">
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A121" s="2" t="s">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A122" s="2" t="s">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A123" s="2" t="s">
+      <c r="B123" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B123" s="2" t="s">
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="B124" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A124" s="2" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B124" s="2" t="s">
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A125" s="2" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A126" s="2" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A127" s="2" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A128" s="2" t="s">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A129" s="2" t="s">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A130" s="2" t="s">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A131" s="2" t="s">
+      <c r="B132" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A132" s="2" t="s">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B132" s="2" t="s">
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A133" s="2" t="s">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A134" s="2" t="s">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A135" s="2" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A136" s="2" t="s">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A137" s="2" t="s">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A138" s="2" t="s">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A139" s="2" t="s">
+      <c r="B140" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A140" s="2" t="s">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B140" s="2" t="s">
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A141" s="2" t="s">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A142" s="2" t="s">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A143" s="2" t="s">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A144" s="2" t="s">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A145" s="2" t="s">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A146" s="2" t="s">
+      <c r="B147" s="3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A147" s="2" t="s">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B147" s="3" t="s">
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A148" s="2" t="s">
+      <c r="B149" s="3" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A149" s="2" t="s">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B149" s="3" t="s">
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A150" s="2" t="s">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A151" s="2" t="s">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A152" s="2" t="s">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A153" s="2" t="s">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A154" s="2" t="s">
+      <c r="B155" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A155" s="2" t="s">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B155" s="2" t="s">
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A156" s="2" t="s">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A157" s="2" t="s">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A158" s="2" t="s">
+      <c r="B159" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A159" s="2" t="s">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B159" s="2" t="s">
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A160" s="2" t="s">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A161" s="2" t="s">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A162" s="2" t="s">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A163" s="2" t="s">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A164" s="2" t="s">
+      <c r="B165" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A165" s="2" t="s">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B165" s="2" t="s">
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A166" s="2" t="s">
+      <c r="B167" s="3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A167" s="2" t="s">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B167" s="3" t="s">
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A168" s="2" t="s">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A169" s="2" t="s">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A170" s="2" t="s">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A171" s="2" t="s">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A172" s="2" t="s">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A173" s="2" t="s">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A174" s="2" t="s">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A175" s="2" t="s">
+      <c r="B176" s="3" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A176" s="2" t="s">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B176" s="3" t="s">
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A177" s="2" t="s">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A178" s="2" t="s">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A179" s="2" t="s">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A180" s="2" t="s">
+      <c r="B181" s="3" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A181" s="2" t="s">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="B181" s="3" t="s">
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A182" s="2" t="s">
+      <c r="B183" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A183" s="2" t="s">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="B183" s="2" t="s">
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A184" s="2" t="s">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A185" s="2" t="s">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A186" s="2" t="s">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A187" s="2" t="s">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A188" s="2" t="s">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A189" s="2" t="s">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A190" s="2" t="s">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A191" s="2" t="s">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="2" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A192" s="2" t="s">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A193" s="2" t="s">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A194" s="2" t="s">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A195" s="2" t="s">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="B195" s="2" t="s">
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A196" s="2" t="s">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" s="2" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A197" s="2" t="s">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A198" s="2" t="s">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A199" s="2" t="s">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A200" s="2" t="s">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A201" s="2" t="s">
+      <c r="B203" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A202" s="2" t="s">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" s="2" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A203" s="2" t="s">
+      <c r="B204" s="3" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A204" s="2" t="s">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B204" s="2" t="s">
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A205" s="2" t="s">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B205" s="3" t="s">
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A206" s="2" t="s">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A207" s="2" t="s">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A208" s="2" t="s">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A209" s="2" t="s">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" s="2" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A210" s="2" t="s">
+      <c r="B212" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A211" s="2" t="s">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A212" s="2" t="s">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" s="2" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A213" s="2" t="s">
+      <c r="B214" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B213" s="2" t="s">
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A214" s="2" t="s">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" s="2" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A215" s="2" t="s">
+      <c r="B216" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="B215" s="2" t="s">
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A216" s="2" t="s">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" s="2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A217" s="2" t="s">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B217" s="3" t="s">
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" s="2" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A218" s="2" t="s">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" s="2" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A219" s="2" t="s">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A220" s="2" t="s">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" s="2" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A221" s="2" t="s">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" s="2" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A222" s="2" t="s">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="2" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A223" s="2" t="s">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A224" s="2" t="s">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="2" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A225" s="2" t="s">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A226" s="2" t="s">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="2" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A227" s="2" t="s">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="2" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A228" s="2" t="s">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="2" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A229" s="2" t="s">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="2" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A230" s="2" t="s">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="2" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A231" s="2" t="s">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A232" s="2" t="s">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="2" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A233" s="2" t="s">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="2" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A234" s="2" t="s">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="2" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A235" s="2" t="s">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="2" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A236" s="2" t="s">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="2" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A237" s="2" t="s">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A238" s="2" t="s">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241" s="2" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A239" s="2" t="s">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242" s="2" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A240" s="2" t="s">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243" s="2" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A241" s="2" t="s">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244" s="2" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A242" s="2" t="s">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245" s="2" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A243" s="2" t="s">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246" s="2" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A244" s="2" t="s">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" s="2" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A245" s="2" t="s">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A246" s="2" t="s">
+      <c r="B248" s="3" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A247" s="2" t="s">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" s="2" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A248" s="2" t="s">
+      <c r="B249" s="2" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A249" s="2" t="s">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B249" s="3" t="s">
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" s="2" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A250" s="2" t="s">
+      <c r="B251" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B250" s="2" t="s">
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" s="2" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A251" s="2" t="s">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" s="2" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A252" s="2" t="s">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="B252" s="2" t="s">
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256" s="2" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A253" s="2" t="s">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="2" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A254" s="2" t="s">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="2" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A256" s="2" t="s">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="2" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A257" s="2" t="s">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" s="2" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A258" s="2" t="s">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="2" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A259" s="2" t="s">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="2" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A260" s="2" t="s">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="2" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A261" s="2" t="s">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="2" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A262" s="2" t="s">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" s="2" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A263" s="2" t="s">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" s="2" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A264" s="2" t="s">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" s="2" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A265" s="2" t="s">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="2" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A266" s="2" t="s">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" s="2" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A267" s="2" t="s">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="2" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A268" s="2" t="s">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" s="2" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A269" s="2" t="s">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" s="2" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A270" s="2" t="s">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" s="2" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A271" s="2" t="s">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" s="2" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A272" s="2" t="s">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="2" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A273" s="2" t="s">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" s="2" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A274" s="2" t="s">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" s="2" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A275" s="2" t="s">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" s="2" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A276" s="2" t="s">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" s="2" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A277" s="2" t="s">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" s="2" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A278" s="2" t="s">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" s="2" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A279" s="2" t="s">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" s="2" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A280" s="2" t="s">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" s="2" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A281" s="2" t="s">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" s="2" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A282" s="2" t="s">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" s="2" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A283" s="2" t="s">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" s="2" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A284" s="2" t="s">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" s="2" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A285" s="2" t="s">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" s="2" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A286" s="2" t="s">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" s="2" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A287" s="2" t="s">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" s="2" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A288" s="2" t="s">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" s="2" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A289" s="2" t="s">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" s="2" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A290" s="2" t="s">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" s="2" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A291" s="2" t="s">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" s="2" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A292" s="2" t="s">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" s="2" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A293" s="2" t="s">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" s="2" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A294" s="2" t="s">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" s="2" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A295" s="2" t="s">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" s="2" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A296" s="2" t="s">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" s="2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A297" s="2" t="s">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" s="2" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A298" s="2" t="s">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" s="2" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A299" s="2" t="s">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" s="2" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A300" s="2" t="s">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A301" s="2" t="s">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" s="2" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A302" s="2" t="s">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" s="2" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A303" s="2" t="s">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" s="2" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A304" s="2" t="s">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" s="2" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A305" s="2" t="s">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" s="2" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A306" s="2" t="s">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" s="2" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A307" s="2" t="s">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" s="2" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A308" s="2" t="s">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" s="2" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A309" s="2" t="s">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" s="2" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A310" s="2" t="s">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" s="2" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A311" s="2" t="s">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" s="2" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A312" s="2" t="s">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" s="2" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A313" s="2" t="s">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A314" s="2" t="s">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A315" s="2" t="s">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" s="2" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A316" s="2" t="s">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" s="2" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A317" s="2" t="s">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320" s="2" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A318" s="2" t="s">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" s="2" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A319" s="2" t="s">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322" s="2" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A320" s="2" t="s">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A323" s="2" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A321" s="2" t="s">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324" s="2" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A322" s="2" t="s">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325" s="2" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A323" s="2" t="s">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326" s="2" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A324" s="2" t="s">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327" s="2" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A325" s="2" t="s">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328" s="2" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A326" s="2" t="s">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329" s="2" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A327" s="2" t="s">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330" s="2" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A328" s="2" t="s">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331" s="2" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A329" s="2" t="s">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332" s="2" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A330" s="2" t="s">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333" s="2" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A331" s="2" t="s">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334" s="2" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A332" s="2" t="s">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335" s="2" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A333" s="2" t="s">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336" s="2" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A334" s="2" t="s">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" s="2" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A335" s="2" t="s">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" s="2" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A336" s="2" t="s">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339" s="2" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A337" s="2" t="s">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340" s="2" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A338" s="2" t="s">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341" s="2" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A339" s="2" t="s">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342" s="2" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A340" s="2" t="s">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343" s="2" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A341" s="2" t="s">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344" s="2" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A342" s="2" t="s">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345" s="2" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A343" s="2" t="s">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346" s="2" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A344" s="2" t="s">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347" s="2" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A345" s="2" t="s">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348" s="2" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A346" s="2" t="s">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349" s="2" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A347" s="2" t="s">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350" s="2" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A348" s="2" t="s">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351" s="2" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A349" s="2" t="s">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352" s="2" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A350" s="2" t="s">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353" s="2" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A351" s="2" t="s">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354" s="2" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A352" s="2" t="s">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355" s="2" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A353" s="2" t="s">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356" s="2" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A354" s="2" t="s">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357" s="2" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A355" s="2" t="s">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358" s="2" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A356" s="2" t="s">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359" s="2" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A357" s="2" t="s">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" s="2" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A358" s="2" t="s">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" s="2" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A359" s="2" t="s">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" s="2" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A360" s="2" t="s">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" s="2" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A361" s="2" t="s">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" s="2" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A362" s="2" t="s">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" s="2" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A363" s="2" t="s">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" s="2" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A364" s="2" t="s">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" s="2" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A365" s="2" t="s">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" s="2" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A366" s="2" t="s">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" s="2" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A367" s="2" t="s">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" s="2" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A368" s="2" t="s">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" s="2" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A369" s="2" t="s">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" s="2" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A370" s="2" t="s">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" s="2" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A371" s="2" t="s">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" s="2" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A372" s="2" t="s">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" s="2" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A373" s="2" t="s">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" s="2" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A374" s="2" t="s">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" s="2" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A375" s="2" t="s">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" s="2" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A376" s="2" t="s">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" s="2" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A377" s="2" t="s">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" s="2" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A378" s="2" t="s">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" s="2" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A379" s="2" t="s">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" s="2" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A380" s="2" t="s">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" s="2" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A381" s="2" t="s">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" s="2" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A382" s="2" t="s">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" s="2" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A383" s="2" t="s">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" s="2" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A384" s="2" t="s">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" s="2" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A385" s="2" t="s">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" s="2" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A386" s="2" t="s">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" s="2" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A387" s="2" t="s">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" s="2" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A388" s="2" t="s">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" s="2" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A389" s="2" t="s">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" s="2" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A390" s="2" t="s">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393" s="2" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A391" s="2" t="s">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394" s="2" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A392" s="2" t="s">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395" s="2" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A393" s="2" t="s">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396" s="2" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A394" s="2" t="s">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397" s="2" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A395" s="2" t="s">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398" s="2" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A396" s="2" t="s">
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A399" s="2" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A397" s="2" t="s">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400" s="2" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A398" s="2" t="s">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401" s="2" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A399" s="2" t="s">
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402" s="2" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A400" s="2" t="s">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" s="2" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A401" s="2" t="s">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" s="2" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A402" s="2" t="s">
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" s="2" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A403" s="2" t="s">
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" s="2" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A404" s="2" t="s">
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" s="2" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A405" s="2" t="s">
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" s="2" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A406" s="2" t="s">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" s="2" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A407" s="2" t="s">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" s="2" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A408" s="2" t="s">
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" s="2" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A409" s="2" t="s">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" s="2" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A410" s="2" t="s">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" s="2" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A411" s="2" t="s">
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" s="2" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A412" s="2" t="s">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" s="2" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A413" s="2" t="s">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" s="2" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A414" s="2" t="s">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" s="2" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A415" s="2" t="s">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" s="2" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A416" s="2" t="s">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" s="2" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A417" s="2" t="s">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" s="2" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A418" s="2" t="s">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" s="2" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A419" s="2" t="s">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" s="2" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A420" s="2" t="s">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" s="2" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A421" s="2" t="s">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" s="2" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A422" s="2" t="s">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" s="2" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A423" s="2" t="s">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" s="2" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A424" s="2" t="s">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" s="2" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A425" s="2" t="s">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" s="2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A426" s="2" t="s">
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" s="2" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A427" s="2" t="s">
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" s="2" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A428" s="2" t="s">
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" s="2" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="429" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A429" s="2" t="s">
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" s="2" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A430" s="2" t="s">
+    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A433" s="2" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A431" s="2" t="s">
+    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A434" s="2" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="432" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A432" s="2" t="s">
+    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A435" s="2" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="433" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A433" s="2" t="s">
+    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A436" s="2" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="434" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A434" s="2" t="s">
+      <c r="B436" s="2" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="435" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A435" s="2" t="s">
+    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A437" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="436" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A436" s="2" t="s">
+    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A438" s="2" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="437" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A437" s="2" t="s">
+    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A439" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="B437" s="2" t="s">
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A440" s="2" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="438" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A438" s="2" t="s">
+    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A441" s="2" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="439" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A439" s="2" t="s">
+    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A442" s="2" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="440" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A440" s="2" t="s">
+    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A443" s="2" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="441" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A441" s="2" t="s">
+    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A444" s="2" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="442" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A442" s="2" t="s">
+    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A445" s="2" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="443" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A443" s="2" t="s">
+    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A446" s="2" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="444" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A444" s="2" t="s">
+    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A447" s="2" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="445" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A445" s="2" t="s">
+    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A448" s="2" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="446" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A446" s="2" t="s">
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" s="2" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="447" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A447" s="2" t="s">
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" s="2" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="448" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A448" s="2" t="s">
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" s="2" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="449" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A449" s="2" t="s">
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" s="2" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="450" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A450" s="2" t="s">
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A453" s="2" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="451" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A451" s="2" t="s">
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A454" s="2" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="452" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A452" s="2" t="s">
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A455" s="2" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="453" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A453" s="2" t="s">
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A456" s="2" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="454" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A454" s="2" t="s">
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A457" s="2" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="455" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A455" s="2" t="s">
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A458" s="2" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="456" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A456" s="2" t="s">
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A459" s="2" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="457" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A457" s="2" t="s">
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A460" s="2" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="458" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A458" s="2" t="s">
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A461" s="2" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="459" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A459" s="2" t="s">
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A462" s="2" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="460" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A460" s="2" t="s">
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A463" s="2" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="461" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A461" s="2" t="s">
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A464" s="2" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="462" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A462" s="2" t="s">
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" s="2" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="463" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A463" s="2" t="s">
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466" s="2" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="464" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A464" s="2" t="s">
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" s="2" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="465" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A465" s="2" t="s">
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" s="2" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="466" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A466" s="2" t="s">
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" s="2" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="467" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A467" s="2" t="s">
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" s="2" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="468" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A468" s="2" t="s">
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" s="2" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="469" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A469" s="2" t="s">
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472" s="2" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="470" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A470" s="2" t="s">
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" s="2" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="471" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A471" s="2" t="s">
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" s="2" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="472" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A472" s="2" t="s">
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" s="2" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="473" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A473" s="2" t="s">
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" s="2" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="474" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A474" s="2" t="s">
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" s="2" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="475" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A475" s="2" t="s">
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" s="2" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="476" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A476" s="2" t="s">
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" s="2" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="477" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A477" s="2" t="s">
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" s="2" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="478" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A478" s="2" t="s">
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" s="2" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="479" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A479" s="2" t="s">
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482" s="2" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="480" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A480" s="2" t="s">
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A483" s="2" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="481" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A481" s="2" t="s">
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A484" s="2" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="482" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A482" s="2" t="s">
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A485" s="2" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="483" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A483" s="2" t="s">
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A486" s="2" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="484" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A484" s="2" t="s">
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A487" s="2" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="485" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A485" s="2" t="s">
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A488" s="2" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="486" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A486" s="2" t="s">
+    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A489" s="2" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="487" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A487" s="2" t="s">
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A490" s="2" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="488" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A488" s="2" t="s">
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A491" s="2" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="489" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A489" s="2" t="s">
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A492" s="2" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="490" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A490" s="2" t="s">
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A493" s="2" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="491" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A491" s="2" t="s">
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A494" s="2" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="492" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A492" s="2" t="s">
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A495" s="2" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="493" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A493" s="2" t="s">
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A496" s="2" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="494" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A494" s="2" t="s">
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A497" s="2" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="495" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A495" s="2" t="s">
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A498" s="2" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="496" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A496" s="2" t="s">
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A499" s="2" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="497" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A497" s="2" t="s">
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A500" s="2" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="498" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A498" s="2" t="s">
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A501" s="2" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="499" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A499" s="2" t="s">
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A502" s="2" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="500" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A500" s="2" t="s">
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A503" s="2" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="501" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A501" s="2" t="s">
+    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A504" s="2" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="502" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A502" s="2" t="s">
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A505" s="2" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="503" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A503" s="2" t="s">
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A506" s="2" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="504" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A504" s="2" t="s">
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A507" s="2" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="505" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A505" s="2" t="s">
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A508" s="2" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="506" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A506" s="2" t="s">
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A509" s="2" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="507" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A507" s="2" t="s">
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A510" s="2" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="508" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A508" s="2" t="s">
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A511" s="2" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="509" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A509" s="2" t="s">
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A512" s="2" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="510" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A510" s="2" t="s">
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A513" s="2" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="511" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A511" s="2" t="s">
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A514" s="2" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="512" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A512" s="2" t="s">
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A515" s="2" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="513" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A513" s="2" t="s">
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A516" s="2" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="514" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A514" s="2" t="s">
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A517" s="2" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="515" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A515" s="2" t="s">
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A518" s="2" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="516" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A516" s="2" t="s">
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A519" s="2" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="517" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A517" s="2" t="s">
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A520" s="2" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="518" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A518" s="2" t="s">
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A521" s="2" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="519" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A519" s="2" t="s">
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A522" s="2" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="520" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A520" s="2" t="s">
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A523" s="2" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="521" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A521" s="2" t="s">
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A524" s="2" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="522" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A522" s="2" t="s">
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A525" s="2" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="523" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A523" s="2" t="s">
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A526" s="2" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="524" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A524" s="2" t="s">
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A527" s="2" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="525" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A525" s="2" t="s">
+    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A528" s="2" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="526" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A526" s="2" t="s">
+    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A529" s="2" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="527" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A527" s="2" t="s">
+    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A530" s="2" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="528" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A528" s="2" t="s">
+    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A531" s="2" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="529" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A529" s="2" t="s">
+    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A532" s="2" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="530" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A530" s="2" t="s">
+    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A533" s="2" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="531" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A531" s="2" t="s">
+    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A534" s="2" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="532" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A532" s="2" t="s">
+    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A535" s="2" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="533" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A533" s="2" t="s">
+    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A536" s="2" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="534" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A534" s="2" t="s">
+    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A537" s="2" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="535" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A535" s="2" t="s">
+    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A538" s="2" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="536" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A536" s="2" t="s">
+    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A539" s="2" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="537" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A537" s="2" t="s">
+    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A540" s="2" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="538" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A538" s="2" t="s">
+    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A541" s="2" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="539" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A539" s="2" t="s">
+    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A542" s="2" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="540" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A540" s="2" t="s">
+    <row r="543" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A543" s="2" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="541" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A541" s="2" t="s">
+    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A544" s="2" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="542" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A542" s="2" t="s">
+    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A545" s="2" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="543" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A543" s="2" t="s">
+    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A546" s="2" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="544" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A544" s="2" t="s">
+    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A547" s="2" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="545" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A545" s="2" t="s">
+    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A548" s="2" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="546" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A546" s="2" t="s">
+    <row r="549" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A549" s="2" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="547" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A547" s="2" t="s">
+    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A550" s="2" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="548" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A548" s="2" t="s">
+    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A551" s="2" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="549" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A549" s="2" t="s">
+    <row r="552" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A552" s="2" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="550" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A550" s="2" t="s">
+    <row r="553" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A553" s="2" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="551" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A551" s="2" t="s">
+    <row r="554" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A554" s="2" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="552" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A552" s="2" t="s">
+    <row r="555" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A555" s="2" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="553" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A553" s="2" t="s">
+    <row r="556" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A556" s="2" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="554" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A554" s="2" t="s">
+    <row r="557" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A557" s="2" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="555" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A555" s="2" t="s">
+    <row r="558" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A558" s="2" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="556" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A556" s="2" t="s">
+    <row r="559" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A559" s="2" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="557" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A557" s="2" t="s">
+    <row r="560" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A560" s="2" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="558" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A558" s="2" t="s">
+    <row r="561" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A561" s="2" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="559" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A559" s="2" t="s">
+    <row r="562" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A562" s="2" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="560" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A560" s="2" t="s">
+    <row r="563" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A563" s="2" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="561" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A561" s="2" t="s">
+    <row r="564" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A564" s="2" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="562" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A562" s="2" t="s">
+    <row r="565" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A565" s="2" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="563" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A563" s="2" t="s">
+    <row r="566" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A566" s="2" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="564" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A564" s="2" t="s">
+    <row r="567" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A567" s="2" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="565" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A565" s="2" t="s">
+    <row r="568" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A568" s="2" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="566" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A566" s="2" t="s">
+    <row r="569" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A569" s="2" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="567" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A567" s="2" t="s">
+    <row r="570" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A570" s="2" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="568" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A568" s="2" t="s">
+    <row r="571" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A571" s="2" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="569" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A569" s="2" t="s">
+    <row r="572" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A572" s="2" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="570" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A570" s="2" t="s">
+    <row r="573" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A573" s="2" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="571" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A571" s="2" t="s">
+    <row r="574" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A574" s="2" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="572" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A572" s="2" t="s">
+    <row r="575" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A575" s="2" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="573" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A573" s="2" t="s">
+    <row r="576" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A576" s="2" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="574" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A574" s="2" t="s">
+    <row r="577" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A577" s="2" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="575" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A575" s="2" t="s">
+    <row r="578" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A578" s="2" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="576" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A576" s="2" t="s">
+    <row r="579" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A579" s="2" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="577" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A577" s="2" t="s">
+    <row r="580" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A580" s="2" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="578" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A578" s="2" t="s">
+    <row r="581" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A581" s="2" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="579" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A579" s="2" t="s">
+    <row r="582" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A582" s="2" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="580" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A580" s="2" t="s">
+    <row r="583" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A583" s="2" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="581" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A581" s="2" t="s">
+    <row r="584" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A584" s="2" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="582" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A582" s="2" t="s">
+    <row r="585" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A585" s="2" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="583" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A583" s="2" t="s">
+    <row r="586" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A586" s="2" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="584" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A584" s="2" t="s">
+    <row r="587" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A587" s="2" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="585" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A585" s="2" t="s">
+    <row r="588" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A588" s="2" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="586" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A586" s="2" t="s">
+    <row r="589" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A589" s="2" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="587" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A587" s="2" t="s">
+    <row r="590" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A590" s="2" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="588" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A588" s="2" t="s">
+    <row r="591" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A591" s="2" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="589" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A589" s="2" t="s">
+    <row r="592" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A592" s="2" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="590" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A590" s="2" t="s">
+    <row r="593" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A593" s="2" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="591" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A591" s="2" t="s">
+    <row r="594" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A594" s="2" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="592" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A592" s="2" t="s">
+    <row r="595" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A595" s="2" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="593" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A593" s="2" t="s">
+    <row r="596" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A596" s="2" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="594" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A594" s="2" t="s">
+    <row r="597" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A597" s="2" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="595" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A595" s="2" t="s">
+    <row r="598" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A598" s="2" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="596" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A596" s="2" t="s">
+    <row r="599" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A599" s="2" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="597" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A597" s="2" t="s">
+    <row r="600" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A600" s="2" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="598" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A598" s="2" t="s">
+    <row r="601" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A601" s="2" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="599" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A599" s="2" t="s">
+    <row r="602" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A602" s="2" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="600" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A600" s="2" t="s">
+    <row r="603" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A603" s="2" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="601" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A601" s="2" t="s">
+    <row r="604" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A604" s="2" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="602" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A602" s="2" t="s">
+    <row r="605" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A605" s="2" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="603" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A603" s="2" t="s">
+    <row r="606" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A606" s="2" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="604" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A604" s="2" t="s">
+    <row r="607" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A607" s="2" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="605" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A605" s="2" t="s">
+    <row r="608" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A608" s="2" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="606" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A606" s="2" t="s">
+    <row r="609" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A609" s="2" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="607" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A607" s="2" t="s">
+    <row r="610" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A610" s="2" t="s">
         <v>670</v>
       </c>
     </row>
-    <row r="608" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A608" s="2" t="s">
+    <row r="611" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A611" s="2" t="s">
         <v>671</v>
       </c>
     </row>
-    <row r="609" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A609" s="2" t="s">
+    <row r="612" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A612" s="2" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="610" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A610" s="2" t="s">
+    <row r="613" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A613" s="2" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="611" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A611" s="2" t="s">
+    <row r="614" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A614" s="2" t="s">
         <v>674</v>
       </c>
     </row>
-    <row r="612" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A612" s="2" t="s">
+    <row r="615" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A615" s="2" t="s">
         <v>675</v>
       </c>
     </row>
-    <row r="613" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A613" s="2" t="s">
+    <row r="616" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A616" s="2" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="614" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A614" s="2" t="s">
+    <row r="617" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A617" s="2" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="615" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A615" s="2" t="s">
+    <row r="618" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A618" s="2" t="s">
         <v>678</v>
       </c>
     </row>
-    <row r="616" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A616" s="2" t="s">
+    <row r="619" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A619" s="2" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="617" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A617" s="2" t="s">
+    <row r="620" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A620" s="2" t="s">
         <v>680</v>
       </c>
     </row>
-    <row r="618" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A618" s="2" t="s">
+    <row r="621" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A621" s="2" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="619" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A619" s="2" t="s">
+    <row r="622" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A622" s="2" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="620" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A620" s="2" t="s">
+    <row r="623" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A623" s="2" t="s">
         <v>683</v>
       </c>
     </row>
-    <row r="621" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A621" s="2" t="s">
+    <row r="624" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A624" s="2" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="622" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A622" s="2" t="s">
+    <row r="625" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A625" s="2" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="623" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A623" s="2" t="s">
+    <row r="626" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A626" s="2" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="624" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A624" s="2" t="s">
+    <row r="627" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A627" s="2" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="625" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A625" s="2" t="s">
+    <row r="628" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A628" s="2" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="626" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A626" s="2" t="s">
+    <row r="629" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A629" s="2" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="627" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A627" s="2" t="s">
+    <row r="630" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A630" s="2" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="628" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A628" s="2" t="s">
+    <row r="631" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A631" s="2" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="629" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A629" s="2" t="s">
+    <row r="632" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A632" s="2" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="630" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A630" s="2" t="s">
+    <row r="633" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A633" s="2" t="s">
         <v>693</v>
       </c>
     </row>
-    <row r="631" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A631" s="2" t="s">
+    <row r="634" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A634" s="2" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="632" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A632" s="2" t="s">
+    <row r="635" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A635" s="2" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="633" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A633" s="2" t="s">
+    <row r="636" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A636" s="2" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="634" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A634" s="2" t="s">
+    <row r="637" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A637" s="2" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="635" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A635" s="2" t="s">
+    <row r="638" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A638" s="2" t="s">
         <v>698</v>
       </c>
     </row>
-    <row r="636" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A636" s="2" t="s">
+    <row r="639" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A639" s="2" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="637" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A637" s="2" t="s">
+    <row r="640" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A640" s="2" t="s">
         <v>700</v>
-      </c>
-    </row>
-    <row r="638" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A638" s="2" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="639" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A639" s="2" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="640" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A640" s="2" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="641" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A641" s="2" t="s">
-        <v>704</v>
       </c>
     </row>
   </sheetData>
@@ -5931,19 +5917,29 @@
     <hyperlink ref="B22" r:id="rId2"/>
     <hyperlink ref="B30" r:id="rId3"/>
     <hyperlink ref="B176" r:id="rId4"/>
-    <hyperlink ref="B205" r:id="rId5"/>
+    <hyperlink ref="B204" r:id="rId5"/>
     <hyperlink ref="B181" r:id="rId6"/>
     <hyperlink ref="B147" r:id="rId7"/>
     <hyperlink ref="B48" r:id="rId8"/>
-    <hyperlink ref="B217" r:id="rId9"/>
+    <hyperlink ref="B216" r:id="rId9"/>
     <hyperlink ref="B167" r:id="rId10"/>
-    <hyperlink ref="B249" r:id="rId11"/>
+    <hyperlink ref="B248" r:id="rId11"/>
+    <hyperlink ref="B16" r:id="rId12"/>
+    <hyperlink ref="B27" r:id="rId13"/>
+    <hyperlink ref="B15" r:id="rId14"/>
+    <hyperlink ref="B3" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101005D3A006B95487C499E3095D35EE726C8" ma:contentTypeVersion="7" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="c8e7208c2fc39913efb382e64ca04520">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e714f09f-c918-41d6-9b18-82b7f6d67f02" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2caf7ad345cd520edfce597314502b8d" ns2:_="">
     <xsd:import namespace="e714f09f-c918-41d6-9b18-82b7f6d67f02"/>
@@ -6107,7 +6103,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -6116,20 +6112,37 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF64FC26-7EC9-475D-BD43-6ADE04953C95}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA37CA62-1189-44A7-8CDD-D01EB1AC2856}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19757496-8AF3-4522-8EC1-01B18DBAE3D4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF64FC26-7EC9-475D-BD43-6ADE04953C95}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e714f09f-c918-41d6-9b18-82b7f6d67f02"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA37CA62-1189-44A7-8CDD-D01EB1AC2856}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19757496-8AF3-4522-8EC1-01B18DBAE3D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>